<commit_message>
Included letter stats for features
</commit_message>
<xml_diff>
--- a/hypertuning_results_wordsonly_1.xlsx
+++ b/hypertuning_results_wordsonly_1.xlsx
@@ -1,20 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agamino/PycharmProjects/pycharm_fellowshipapi/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView xWindow="240" yWindow="680" windowWidth="28560" windowHeight="17380"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Results" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>a_number_of_documents</t>
   </si>
@@ -73,23 +86,24 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -104,26 +118,40 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -411,20 +439,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.83203125" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -468,35 +498,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>1000</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2">
         <v>400</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>100</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>14003</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="n">
-        <v>36.57142857142857</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G2">
+        <v>36.571428571428569</v>
+      </c>
+      <c r="H2">
         <v>21000</v>
       </c>
-      <c r="I2" t="n">
+      <c r="I2">
         <v>16800</v>
       </c>
-      <c r="J2" t="n">
+      <c r="J2">
         <v>4200</v>
       </c>
       <c r="K2" t="s">
@@ -511,11 +541,11 @@
       <c r="N2" t="s">
         <v>14</v>
       </c>
-      <c r="O2" t="n">
+      <c r="O2">
         <v>0.664047619047619</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>